<commit_message>
Update OpenAI news: 2026-01-27 01:12:34
</commit_message>
<xml_diff>
--- a/openai_news.xlsx
+++ b/openai_news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,141 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>글로벌(OpenAI)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>How Indeed uses AI to help evolve the job search</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mon, 26 Jan 2026 00:00:00 GMT</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://openai.com/index/indeed-maggie-hulce</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>글로벌(OpenAI)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Unrolling the Codex agent loop</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Fri, 23 Jan 2026 12:00:00 GMT</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://openai.com/index/unrolling-the-codex-agent-loop</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>글로벌(OpenAI)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Scaling PostgreSQL to power 800 million ChatGPT users</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Thu, 22 Jan 2026 12:00:00 GMT</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://openai.com/index/scaling-postgresql</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>글로벌(OpenAI)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Inside Praktika's conversational approach to language learning</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Thu, 22 Jan 2026 05:00:00 GMT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://openai.com/index/praktika</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>글로벌(OpenAI)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Inside GPT-5 for Work: How Businesses Use GPT-5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Thu, 22 Jan 2026 00:00:00 GMT</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://openai.com/business/guides-and-resources/chatgpt-usage-and-adoption-patterns-at-work</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update OpenAI news (with translation)
</commit_message>
<xml_diff>
--- a/openai_news.xlsx
+++ b/openai_news.xlsx
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>수집일</t>
+          <t>발행일</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>카테고리</t>
+          <t>기관</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>기사제목</t>
+          <t>원문 제목</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>발행일</t>
+          <t>한글 번역 제목</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>글로벌(OpenAI)</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mon, 26 Jan 2026 00:00:00 GMT</t>
+          <t>인디드가 AI를 활용하여 구직 활동을 발전시키는 방법</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>글로벌(OpenAI)</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Fri, 23 Jan 2026 12:00:00 GMT</t>
+          <t>Codex 에이전트 루프 풀기</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -517,12 +517,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>글로벌(OpenAI)</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Thu, 22 Jan 2026 12:00:00 GMT</t>
+          <t>PostgreSQL을 확장하여 8억 명의 ChatGPT 사용자 지원</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,12 +544,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>글로벌(OpenAI)</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Thu, 22 Jan 2026 05:00:00 GMT</t>
+          <t>Praktika의 언어 학습에 대한 대화식 접근 방식 살펴보기</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -571,12 +571,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>글로벌(OpenAI)</t>
+          <t>OpenAI</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Thu, 22 Jan 2026 00:00:00 GMT</t>
+          <t>업무용 GPT-5 내부: 기업이 GPT-5를 사용하는 방법</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">

</xml_diff>